<commit_message>
updated files for macrofab
</commit_message>
<xml_diff>
--- a/modules/microwave_radar/hardware/rev_b/macrofab_compliant/microwave_bom.xlsx
+++ b/modules/microwave_radar/hardware/rev_b/macrofab_compliant/microwave_bom.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="microwave_part_bom" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="microwave_bom" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="257">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -235,6 +235,12 @@
     <t xml:space="preserve">C20</t>
   </si>
   <si>
+    <t xml:space="preserve">C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22</t>
+  </si>
+  <si>
     <t xml:space="preserve">6.8uF</t>
   </si>
   <si>
@@ -250,7 +256,7 @@
     <t xml:space="preserve">C1608X5R1A685K080AC</t>
   </si>
   <si>
-    <t xml:space="preserve">C21</t>
+    <t xml:space="preserve">C23</t>
   </si>
   <si>
     <t xml:space="preserve">10uF</t>
@@ -274,7 +280,7 @@
     <t xml:space="preserve">C0805C106K8PACTU</t>
   </si>
   <si>
-    <t xml:space="preserve">C22</t>
+    <t xml:space="preserve">C24</t>
   </si>
   <si>
     <t xml:space="preserve">22uF</t>
@@ -292,7 +298,7 @@
     <t xml:space="preserve">CC0603MRX5R5BB226</t>
   </si>
   <si>
-    <t xml:space="preserve">C23</t>
+    <t xml:space="preserve">C25</t>
   </si>
   <si>
     <t xml:space="preserve">100uF</t>
@@ -331,18 +337,6 @@
     <t xml:space="preserve">BLM18HE152SN1D</t>
   </si>
   <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUMPER-2PTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1X02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumper</t>
-  </si>
-  <si>
     <t xml:space="preserve">J3</t>
   </si>
   <si>
@@ -463,33 +457,12 @@
     <t xml:space="preserve">LTST-C191KGKT</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI223DDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6A SOT-23 P Fet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI2333DDS-T1-GE3CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Siliconix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI2333DDS-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1</t>
   </si>
   <si>
+    <t xml:space="preserve">DNP - 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">RESISTOR0402_RES</t>
   </si>
   <si>
@@ -523,72 +496,72 @@
     <t xml:space="preserve">R3</t>
   </si>
   <si>
+    <t xml:space="preserve">8.2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 8.2K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-8.20KLRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-078K2L</t>
+  </si>
+  <si>
     <t xml:space="preserve">R4</t>
   </si>
   <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 10K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-3431-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC1005F103CS</t>
+  </si>
+  <si>
     <t xml:space="preserve">R5</t>
   </si>
   <si>
-    <t xml:space="preserve">8.2k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 8.2K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-8.20KLRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-078K2L</t>
-  </si>
-  <si>
     <t xml:space="preserve">R6</t>
   </si>
   <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 10K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-3431-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1005F103CS</t>
+    <t xml:space="preserve">12k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 12K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-4122-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC1005F123CS</t>
   </si>
   <si>
     <t xml:space="preserve">R7</t>
   </si>
   <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 100K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-3432-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC1005F104CS</t>
+  </si>
+  <si>
     <t xml:space="preserve">R8</t>
   </si>
   <si>
-    <t xml:space="preserve">12k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 12K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-4122-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1005F123CS</t>
-  </si>
-  <si>
     <t xml:space="preserve">R9</t>
   </si>
   <si>
-    <t xml:space="preserve">100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 100K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-3432-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1005F104CS</t>
-  </si>
-  <si>
     <t xml:space="preserve">R10</t>
   </si>
   <si>
@@ -604,85 +577,103 @@
     <t xml:space="preserve">R14</t>
   </si>
   <si>
+    <t xml:space="preserve">200k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR0603_RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603-RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 200K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-200KGRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603JR-07200KL</t>
+  </si>
+  <si>
     <t xml:space="preserve">R15</t>
   </si>
   <si>
+    <t xml:space="preserve">240k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 240K OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P240KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF2403X</t>
+  </si>
+  <si>
     <t xml:space="preserve">R16</t>
   </si>
   <si>
-    <t xml:space="preserve">200k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESISTOR0603_RES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603-RES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 200K OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-200KGRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603JR-07200KL</t>
+    <t xml:space="preserve">330k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 330K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-4244-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC1005F334CS</t>
   </si>
   <si>
     <t xml:space="preserve">R17</t>
   </si>
   <si>
-    <t xml:space="preserve">240k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 240K OHM 1% 1/10W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P240KLCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panasonic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-2RKF2403X</t>
+    <t xml:space="preserve">750k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 750K OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P750KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF7503X</t>
   </si>
   <si>
     <t xml:space="preserve">R18</t>
   </si>
   <si>
-    <t xml:space="preserve">330k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 330K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-4244-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1005F334CS</t>
+    <t xml:space="preserve">1M</t>
   </si>
   <si>
     <t xml:space="preserve">R19</t>
   </si>
   <si>
-    <t xml:space="preserve">750k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES SMD 750K OHM 1% 1/10W 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P750KLCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-2RKF7503X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R21</t>
+    <t xml:space="preserve">S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIP3240X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDFN4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High power (2.4 A) high-side switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIP32402ADNP-T1GE4CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIP32402ADNP-T1GE4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -895,7 +886,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -907,7 +898,7 @@
     <col collapsed="false" hidden="false" max="4" min="2" style="0" width="28.1071428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="67.7040816326531"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0255102040816"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8010204081633"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.4081632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
@@ -1498,65 +1489,65 @@
         <v>70</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>21</v>
@@ -1568,382 +1559,403 @@
         <v>13</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>103</v>
+        <v>92</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>106</v>
+        <v>13</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>109</v>
+        <v>12</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>121</v>
+        <v>114</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>115</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>1212</v>
+        <v>125</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>1212</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>150</v>
+        <v>140</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>141</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="D35" s="0" t="s">
+      <c r="E35" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="G35" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="H35" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" s="0" t="s">
+      <c r="H36" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,28 +1963,28 @@
         <v>167</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H39" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,13 +1995,13 @@
         <v>169</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>170</v>
@@ -1998,7 +2010,7 @@
         <v>171</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>172</v>
@@ -2012,13 +2024,13 @@
         <v>174</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>175</v>
@@ -2041,13 +2053,13 @@
         <v>174</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>175</v>
@@ -2067,561 +2079,526 @@
         <v>179</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H43" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H44" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H45" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H46" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H47" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>185</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>186</v>
-      </c>
       <c r="G49" s="0" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="H50" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="H51" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="I51" s="0" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>206</v>
+        <v>66</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="C53" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="H53" s="0" t="s">
         <v>66</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="G54" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F54" s="0" t="s">
+      <c r="H54" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="G54" s="0" t="s">
+      <c r="I54" s="0" t="s">
         <v>216</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>219</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>157</v>
+        <v>220</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>66</v>
+        <v>223</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>234</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>247</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H61" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="I61" s="0" t="s">
         <v>252</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>